<commit_message>
Regione: REGIONE_CAMPANIA, ASL: ASL_NA_1_NORD, Issuer: integrity:S1#VICAMPANIA1NORD
</commit_message>
<xml_diff>
--- a/REGIONE_CAMPANIA/ASL_NA_1_NORD/integrity:S1#VICAMPANIA1NORD.xlsx
+++ b/REGIONE_CAMPANIA/ASL_NA_1_NORD/integrity:S1#VICAMPANIA1NORD.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -35,16 +35,19 @@
     <t>Creazione_0</t>
   </si>
   <si>
+    <t>REGIONE_LAZIO</t>
+  </si>
+  <si>
     <t>MRCLSN97C14H501J^^^&amp;2.16.840.1.113883.2.9.4.3.2&amp;ISO</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.ff6ce61428^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.f73afc3a33^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721652226262</t>
+    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721654256960</t>
   </si>
   <si>
-    <t>22-07-2024:14:43:47</t>
+    <t>22-07-2024:15:17:38</t>
   </si>
 </sst>
 </file>
@@ -119,18 +122,20 @@
       <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" s="0"/>
-      <c r="C2" t="s" s="0">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="D2" t="s" s="0">
         <v>9</v>
       </c>
+      <c r="E2" t="s" s="0">
+        <v>10</v>
+      </c>
       <c r="F2" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>